<commit_message>
Updated User ID & Password
</commit_message>
<xml_diff>
--- a/com.internetBanking/TestData/TestData.xlsx
+++ b/com.internetBanking/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15525" windowHeight="6540" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15030" windowHeight="6540"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1:J20"/>
 </workbook>
 </file>
 
@@ -28,12 +29,6 @@
     <t>ExpTitle</t>
   </si>
   <si>
-    <t>mngr511658</t>
-  </si>
-  <si>
-    <t>gAdejyz</t>
-  </si>
-  <si>
     <t>https://demo.guru99.com/v4/</t>
   </si>
   <si>
@@ -176,6 +171,12 @@
   </si>
   <si>
     <t>aksh@23</t>
+  </si>
+  <si>
+    <t>mngr516795</t>
+  </si>
+  <si>
+    <t>hYtYvYz</t>
   </si>
 </sst>
 </file>
@@ -524,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -548,13 +549,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -567,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -585,31 +586,31 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
       </c>
       <c r="J1" t="s">
         <v>1</v>
@@ -617,22 +618,22 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1">
         <v>44002</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
       </c>
       <c r="G2">
         <v>413006</v>
@@ -641,30 +642,30 @@
         <v>9852636225</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>44368</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
       </c>
       <c r="G3">
         <v>413006</v>
@@ -673,30 +674,30 @@
         <v>9852636226</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1">
         <v>44734</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
         <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
       </c>
       <c r="G4">
         <v>413006</v>
@@ -705,10 +706,10 @@
         <v>9852636227</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -746,31 +747,31 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
       </c>
       <c r="J1" t="s">
         <v>1</v>
@@ -778,98 +779,98 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1">
         <v>34658</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>35165</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
         <v>34629</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -903,130 +904,130 @@
   <sheetData>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>34658</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
         <v>35165</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1">
         <v>34629</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1">
         <v>34831</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>